<commit_message>
use to_bool method of WorksheetImporter in Product import for hazardous
- change validation for 'hazardous' column of Products sheet in test.xlsx to take values from boolean column in constants sheet.
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test/test.xlsx
+++ b/bika/lims/setupdata/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="51"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="51"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3993" uniqueCount="1615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3987" uniqueCount="1613">
   <si>
     <t>Instructions</t>
   </si>
@@ -3876,9 +3876,6 @@
     <t>30308ss</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Transfer pipette</t>
   </si>
   <si>
@@ -3913,9 +3910,6 @@
   </si>
   <si>
     <t>323</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>Sulfuric acid and other acids are very corrosive and irritating and cause direct local effects on the skin, eyes, and respiratory and gastrointestinal tracts when there is direct exposure to sufficient concentrations. Breathing sulfuric acid mists can result in tooth erosion and respiratory tract irritation. Drinking concentrated sulfuric acid can burn your mouth and throat, and it can erode a hole in your stomach; it has also resulted in death. If you touch sulfuric acid, it will burn your skin. If you get sulfuric acid in your eyes, it will burn your eyes and cause them to water. The term "burn" used in these sections refers to a chemical burn, not a physical burn resulting from contacting a hot object. People have been blinded by sulfuric acid when it was thrown in their faces.</t>
@@ -5346,7 +5340,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="174">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5963,10 +5957,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -12184,7 +12174,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -17422,7 +17412,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="false" error="Select a valid entry from the drop down list." errorTitle="Invalid Analysis Service" operator="equal" prompt="Select an Analysis Service  from the list. Maintain the list on the 'Analysis Services' sheet" promptTitle="Select an Analysis Service" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A103" type="list">
-      <formula1>'Analysis Services'!$A$4:$A$141</formula1>
+      <formula1>'analysis services'!$a$4:$a$141</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -25635,7 +25625,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="false" error="Select a valid Analysis Service from the selection list" errorTitle="Invalid entry" operator="equal" prompt="From the selection list. Populate the selection list on the 'Analysis Services' sheet" promptTitle="Select a valid Analysis Service" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B4:B10" type="list">
-      <formula1>'analysis services'!$a$4:$a$102</formula1>
+      <formula1>'Analysis Services'!$A$4:$A$102</formula1>
       <formula2>h</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A4:A10" type="list">
@@ -25661,7 +25651,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -25791,7 +25781,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="false" error="Select a valid Analysis Service from the selection list" errorTitle="Invalid entry" operator="equal" prompt="From the selection list. Populate the selection list on the 'Analysis Services' sheet" promptTitle="Select a valid Analysis Service" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A10 D4:D10" type="list">
-      <formula1>'analysis services'!$a$4:$a$102</formula1>
+      <formula1>'Analysis Services'!$A$4:$A$102</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -26190,7 +26180,7 @@
   <dimension ref="1:12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -26358,8 +26348,8 @@
       <c r="F4" s="103" t="s">
         <v>1228</v>
       </c>
-      <c r="G4" s="154" t="s">
-        <v>1229</v>
+      <c r="G4" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="H4" s="100"/>
       <c r="I4" s="104"/>
@@ -26381,7 +26371,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="101" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="C5" s="102" t="s">
         <v>1204</v>
@@ -26391,10 +26381,10 @@
       </c>
       <c r="E5" s="103"/>
       <c r="F5" s="103" t="s">
-        <v>1231</v>
-      </c>
-      <c r="G5" s="154" t="s">
-        <v>1229</v>
+        <v>1230</v>
+      </c>
+      <c r="G5" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="H5" s="100"/>
       <c r="I5" s="104"/>
@@ -26416,7 +26406,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="101" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="C6" s="102" t="s">
         <v>1204</v>
@@ -26426,10 +26416,10 @@
       </c>
       <c r="E6" s="103"/>
       <c r="F6" s="103" t="s">
-        <v>1233</v>
-      </c>
-      <c r="G6" s="154" t="s">
-        <v>1229</v>
+        <v>1232</v>
+      </c>
+      <c r="G6" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="H6" s="100" t="n">
         <v>50</v>
@@ -26453,7 +26443,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="101" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C7" s="102" t="s">
         <v>1204</v>
@@ -26463,9 +26453,11 @@
       </c>
       <c r="E7" s="103"/>
       <c r="F7" s="103" t="s">
-        <v>1235</v>
-      </c>
-      <c r="G7" s="154"/>
+        <v>1234</v>
+      </c>
+      <c r="G7" s="22" t="n">
+        <v>0</v>
+      </c>
       <c r="H7" s="100" t="n">
         <v>100</v>
       </c>
@@ -26488,7 +26480,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="101" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="102" t="s">
@@ -26499,9 +26491,11 @@
       </c>
       <c r="E8" s="103"/>
       <c r="F8" s="103" t="s">
-        <v>1237</v>
-      </c>
-      <c r="G8" s="154"/>
+        <v>1236</v>
+      </c>
+      <c r="G8" s="22" t="n">
+        <v>0</v>
+      </c>
       <c r="H8" s="100" t="n">
         <v>2</v>
       </c>
@@ -26524,7 +26518,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="101" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="102" t="s">
@@ -26537,7 +26531,9 @@
       <c r="F9" s="103" t="n">
         <v>2323</v>
       </c>
-      <c r="G9" s="154"/>
+      <c r="G9" s="22" t="n">
+        <v>0</v>
+      </c>
       <c r="H9" s="100"/>
       <c r="I9" s="104"/>
       <c r="J9" s="105" t="n">
@@ -26558,7 +26554,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="21" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="102" t="s">
@@ -26568,13 +26564,13 @@
         <v>621</v>
       </c>
       <c r="E10" s="21" t="s">
+        <v>1239</v>
+      </c>
+      <c r="F10" s="21" t="s">
         <v>1240</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>1241</v>
-      </c>
-      <c r="G10" s="154" t="s">
-        <v>1242</v>
+      <c r="G10" s="22" t="n">
+        <v>1</v>
       </c>
       <c r="H10" s="100" t="n">
         <v>1231.5</v>
@@ -26589,11 +26585,11 @@
         <v>12.11</v>
       </c>
       <c r="L10" s="100"/>
-      <c r="M10" s="155" t="s">
-        <v>1243</v>
+      <c r="M10" s="154" t="s">
+        <v>1241</v>
       </c>
       <c r="N10" s="105" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="P10" s="21"/>
       <c r="Q10" s="66"/>
@@ -26603,7 +26599,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="21" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="102" t="s">
@@ -26613,13 +26609,13 @@
         <v>621</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>1247</v>
-      </c>
-      <c r="G11" s="154" t="s">
-        <v>1242</v>
+        <v>1245</v>
+      </c>
+      <c r="G11" s="22" t="n">
+        <v>1</v>
       </c>
       <c r="H11" s="100"/>
       <c r="I11" s="104"/>
@@ -26627,14 +26623,14 @@
       <c r="K11" s="105" t="n">
         <v>12.11</v>
       </c>
-      <c r="L11" s="156" t="s">
-        <v>1248</v>
-      </c>
-      <c r="M11" s="155" t="s">
-        <v>1249</v>
+      <c r="L11" s="155" t="s">
+        <v>1246</v>
+      </c>
+      <c r="M11" s="154" t="s">
+        <v>1247</v>
       </c>
       <c r="N11" s="105" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="P11" s="21"/>
       <c r="Q11" s="66"/>
@@ -26644,7 +26640,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="21" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="102" t="s">
@@ -26654,13 +26650,13 @@
         <v>621</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>1252</v>
-      </c>
-      <c r="G12" s="154" t="s">
-        <v>1229</v>
+        <v>1250</v>
+      </c>
+      <c r="G12" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="H12" s="100"/>
       <c r="I12" s="100"/>
@@ -26668,11 +26664,11 @@
       <c r="K12" s="105" t="n">
         <v>12.11</v>
       </c>
-      <c r="L12" s="156" t="s">
-        <v>1253</v>
+      <c r="L12" s="155" t="s">
+        <v>1251</v>
       </c>
       <c r="M12" s="105" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="N12" s="105"/>
       <c r="P12" s="21"/>
@@ -26682,13 +26678,13 @@
       <c r="T12" s="18"/>
     </row>
   </sheetData>
-  <dataValidations count="8">
+  <dataValidations count="9">
+    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G5:G12" type="list">
+      <formula1>Constants!$G$2:$G$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="false" error="Select a valid entry from the drop down list." errorTitle="Invalid Supplier" operator="equal" prompt="Select a Supplier from the list. Maintain the list on the 'Suppliers' sheet" promptTitle="Select a Supplier" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D12" type="list">
       <formula1>Suppliers!$A$4:$A$200</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G4:G12" type="list">
-      <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" prompt="No" promptTitle="Default value" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G3" type="none">
@@ -26713,6 +26709,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="greaterThan" prompt="Use . (dot) as delimiter" promptTitle="Quantity in Decimal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H12" type="none">
       <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G4" type="list">
+      <formula1>Constants!$G$2:$G$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -26754,7 +26754,7 @@
     </row>
     <row r="2" s="37" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="C2" s="7"/>
     </row>
@@ -26768,34 +26768,34 @@
     </row>
     <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="66" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="66" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="B5" s="66" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="66" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="B6" s="66" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="66" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="B7" s="66" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
     </row>
   </sheetData>
@@ -26846,10 +26846,10 @@
         <v>302</v>
       </c>
       <c r="C1" s="66" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="E1" s="66" t="s">
         <v>1168</v>
@@ -26864,19 +26864,19 @@
         <v>1172</v>
       </c>
       <c r="I1" s="66" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="J1" s="66" t="s">
         <v>528</v>
       </c>
       <c r="K1" s="66" t="s">
+        <v>1265</v>
+      </c>
+      <c r="L1" s="66" t="s">
+        <v>1266</v>
+      </c>
+      <c r="M1" s="66" t="s">
         <v>1267</v>
-      </c>
-      <c r="L1" s="66" t="s">
-        <v>1268</v>
-      </c>
-      <c r="M1" s="66" t="s">
-        <v>1269</v>
       </c>
       <c r="N1" s="66" t="s">
         <v>827</v>
@@ -26884,22 +26884,22 @@
     </row>
     <row r="2" s="37" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="C2" s="7"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="157" t="s">
-        <v>1271</v>
+      <c r="A3" s="156" t="s">
+        <v>1269</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>439</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>1180</v>
@@ -26914,25 +26914,25 @@
         <v>1184</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>528</v>
       </c>
       <c r="K3" s="6" t="s">
+        <v>1273</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>1274</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>1275</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>1276</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>1277</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>827</v>
       </c>
-      <c r="AMI3" s="157"/>
-      <c r="AMJ3" s="157"/>
+      <c r="AMI3" s="156"/>
+      <c r="AMJ3" s="156"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -26953,7 +26953,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -26976,31 +26976,31 @@
         <v>1163</v>
       </c>
       <c r="B1" s="66" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="C1" s="66" t="s">
         <v>302</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>1277</v>
+      </c>
+      <c r="E1" s="66" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F1" s="66" t="s">
         <v>1279</v>
-      </c>
-      <c r="E1" s="66" t="s">
-        <v>1280</v>
-      </c>
-      <c r="F1" s="66" t="s">
-        <v>1281</v>
       </c>
       <c r="G1" s="66" t="s">
         <v>1123</v>
       </c>
       <c r="H1" s="66" t="s">
+        <v>1280</v>
+      </c>
+      <c r="I1" s="66" t="s">
+        <v>1281</v>
+      </c>
+      <c r="J1" s="66" t="s">
         <v>1282</v>
-      </c>
-      <c r="I1" s="66" t="s">
-        <v>1283</v>
-      </c>
-      <c r="J1" s="66" t="s">
-        <v>1284</v>
       </c>
       <c r="K1" s="66" t="s">
         <v>965</v>
@@ -27009,7 +27009,7 @@
         <v>1169</v>
       </c>
       <c r="M1" s="66" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="N1" s="66" t="s">
         <v>827</v>
@@ -27017,49 +27017,49 @@
     </row>
     <row r="2" s="37" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="B2" s="7"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>439</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>1286</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>1287</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>1288</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>1289</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>1290</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>1291</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>1292</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>1293</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>1294</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>1295</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>1181</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>827</v>
@@ -27105,7 +27105,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="21.65" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1163</v>
@@ -27120,7 +27120,7 @@
         <v>1162</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>1189</v>
@@ -27172,7 +27172,7 @@
         <v>1162</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>1198</v>
@@ -27187,13 +27187,13 @@
         <v>1191</v>
       </c>
       <c r="K3" s="6" t="s">
+        <v>1297</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>1298</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>1299</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>1300</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>1301</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -27319,7 +27319,7 @@
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="26.4" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>939</v>
@@ -27339,13 +27339,13 @@
     </row>
     <row r="2" s="37" customFormat="true" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="C2" s="7"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>944</v>
@@ -27406,7 +27406,7 @@
     </row>
     <row r="2" s="37" customFormat="true" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="C2" s="7"/>
     </row>
@@ -27423,12 +27423,12 @@
     </row>
     <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="66" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>1307</v>
-      </c>
-      <c r="C4" s="158" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C4" s="157" t="s">
         <v>654</v>
       </c>
     </row>
@@ -27472,7 +27472,7 @@
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1108</v>
@@ -27480,29 +27480,29 @@
     </row>
     <row r="2" s="37" customFormat="true" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="C2" s="7"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>1135</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="158" t="s">
-        <v>1306</v>
+      <c r="A4" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B4" s="84" t="s">
         <v>1004</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="158" t="s">
-        <v>1306</v>
+      <c r="A5" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B5" s="84" t="s">
         <v>1017</v>
@@ -27717,53 +27717,53 @@
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>883</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>1310</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1311</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>1312</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>1313</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>1314</v>
       </c>
     </row>
     <row r="2" s="37" customFormat="true" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="C2" s="7"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>656</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>1317</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>1318</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>1319</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>1320</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="158" t="s">
-        <v>1306</v>
+      <c r="A4" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B4" s="8" t="n">
         <v>1</v>
@@ -27778,14 +27778,14 @@
       <c r="F4" s="84"/>
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="158" t="s">
-        <v>1306</v>
+      <c r="A5" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B5" s="8" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="84" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="D5" s="84"/>
       <c r="E5" s="84" t="s">
@@ -27794,224 +27794,224 @@
       <c r="F5" s="84"/>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="158" t="s">
-        <v>1306</v>
+      <c r="A6" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B6" s="8" t="n">
         <v>3</v>
       </c>
       <c r="C6" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D6" s="84"/>
       <c r="E6" s="84"/>
       <c r="F6" s="84"/>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="158" t="s">
-        <v>1306</v>
+      <c r="A7" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B7" s="8" t="n">
         <v>4</v>
       </c>
       <c r="C7" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D7" s="84"/>
       <c r="E7" s="84"/>
       <c r="F7" s="84"/>
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="158" t="s">
-        <v>1306</v>
+      <c r="A8" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B8" s="8" t="n">
         <v>5</v>
       </c>
       <c r="C8" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D8" s="84"/>
       <c r="E8" s="84"/>
       <c r="F8" s="84"/>
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="158" t="s">
-        <v>1306</v>
+      <c r="A9" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B9" s="8" t="n">
         <v>6</v>
       </c>
       <c r="C9" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D9" s="84"/>
       <c r="E9" s="84"/>
       <c r="F9" s="84"/>
     </row>
     <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="158" t="s">
-        <v>1306</v>
+      <c r="A10" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B10" s="8" t="n">
         <v>7</v>
       </c>
       <c r="C10" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D10" s="84"/>
       <c r="E10" s="84"/>
       <c r="F10" s="84"/>
     </row>
     <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="158" t="s">
-        <v>1306</v>
+      <c r="A11" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B11" s="8" t="n">
         <v>8</v>
       </c>
       <c r="C11" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D11" s="84"/>
       <c r="E11" s="84"/>
       <c r="F11" s="84"/>
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="158" t="s">
-        <v>1306</v>
+      <c r="A12" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B12" s="8" t="n">
         <v>9</v>
       </c>
       <c r="C12" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D12" s="84"/>
       <c r="E12" s="84"/>
       <c r="F12" s="84"/>
     </row>
     <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="158" t="s">
-        <v>1306</v>
+      <c r="A13" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B13" s="8" t="n">
         <v>10</v>
       </c>
       <c r="C13" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D13" s="84"/>
       <c r="E13" s="84"/>
       <c r="F13" s="84"/>
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="158" t="s">
-        <v>1306</v>
+      <c r="A14" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B14" s="8" t="n">
         <v>11</v>
       </c>
       <c r="C14" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D14" s="84"/>
       <c r="E14" s="84"/>
       <c r="F14" s="84"/>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="158" t="s">
-        <v>1306</v>
+      <c r="A15" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B15" s="8" t="n">
         <v>12</v>
       </c>
       <c r="C15" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D15" s="84"/>
       <c r="E15" s="84"/>
       <c r="F15" s="84"/>
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="158" t="s">
-        <v>1306</v>
+      <c r="A16" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B16" s="8" t="n">
         <v>13</v>
       </c>
       <c r="C16" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D16" s="84"/>
       <c r="E16" s="84"/>
       <c r="F16" s="84"/>
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="158" t="s">
-        <v>1306</v>
+      <c r="A17" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B17" s="8" t="n">
         <v>14</v>
       </c>
       <c r="C17" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D17" s="84"/>
       <c r="E17" s="84"/>
       <c r="F17" s="84"/>
     </row>
     <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="158" t="s">
-        <v>1306</v>
+      <c r="A18" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B18" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C18" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D18" s="84"/>
       <c r="E18" s="84"/>
       <c r="F18" s="84"/>
     </row>
     <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="158" t="s">
-        <v>1306</v>
+      <c r="A19" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B19" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C19" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D19" s="84"/>
       <c r="E19" s="84"/>
       <c r="F19" s="84"/>
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="158" t="s">
-        <v>1306</v>
+      <c r="A20" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B20" s="8" t="n">
         <v>17</v>
       </c>
       <c r="C20" s="84" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D20" s="84"/>
       <c r="E20" s="84"/>
       <c r="F20" s="84"/>
     </row>
     <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="158" t="s">
-        <v>1306</v>
+      <c r="A21" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B21" s="8" t="n">
         <v>18</v>
       </c>
       <c r="C21" s="84" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="D21" s="84"/>
       <c r="E21" s="84"/>
@@ -28020,14 +28020,14 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="158" t="s">
-        <v>1306</v>
+      <c r="A22" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B22" s="8" t="n">
         <v>19</v>
       </c>
       <c r="C22" s="84" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="D22" s="84"/>
       <c r="E22" s="84" t="s">
@@ -28036,8 +28036,8 @@
       <c r="F22" s="84"/>
     </row>
     <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="158" t="s">
-        <v>1306</v>
+      <c r="A23" s="157" t="s">
+        <v>1304</v>
       </c>
       <c r="B23" s="8" t="n">
         <v>20</v>
@@ -28120,15 +28120,15 @@
       <c r="B1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="159" t="s">
+      <c r="C1" s="158" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="true" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="7" t="s">
-        <v>1323</v>
-      </c>
-      <c r="C2" s="160"/>
+        <v>1321</v>
+      </c>
+      <c r="C2" s="159"/>
     </row>
     <row r="3" s="5" customFormat="true" ht="12.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
@@ -28137,73 +28137,73 @@
       <c r="B3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="159" t="s">
+      <c r="C3" s="158" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="B4" s="137" t="s">
-        <v>1325</v>
-      </c>
-      <c r="C4" s="161" t="n">
+        <v>1323</v>
+      </c>
+      <c r="C4" s="160" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="B5" s="137" t="s">
-        <v>1327</v>
-      </c>
-      <c r="C5" s="161" t="n">
+        <v>1325</v>
+      </c>
+      <c r="C5" s="160" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="B6" s="137" t="s">
-        <v>1328</v>
-      </c>
-      <c r="C6" s="161" t="s">
-        <v>1329</v>
+        <v>1326</v>
+      </c>
+      <c r="C6" s="160" t="s">
+        <v>1327</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="B7" s="137" t="s">
-        <v>1331</v>
-      </c>
-      <c r="C7" s="162" t="n">
+        <v>1329</v>
+      </c>
+      <c r="C7" s="161" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="B8" s="137" t="s">
-        <v>1333</v>
-      </c>
-      <c r="C8" s="162" t="n">
+        <v>1331</v>
+      </c>
+      <c r="C8" s="161" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="B9" s="137" t="s">
-        <v>1335</v>
-      </c>
-      <c r="C9" s="161" t="n">
+        <v>1333</v>
+      </c>
+      <c r="C9" s="160" t="n">
         <v>15</v>
       </c>
     </row>
@@ -28212,230 +28212,230 @@
         <v>226</v>
       </c>
       <c r="B10" s="137" t="s">
-        <v>1336</v>
-      </c>
-      <c r="C10" s="161" t="n">
+        <v>1334</v>
+      </c>
+      <c r="C10" s="160" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="B11" s="137" t="s">
-        <v>1338</v>
-      </c>
-      <c r="C11" s="161" t="n">
+        <v>1336</v>
+      </c>
+      <c r="C11" s="160" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="B12" s="137" t="s">
-        <v>1340</v>
-      </c>
-      <c r="C12" s="161" t="n">
+        <v>1338</v>
+      </c>
+      <c r="C12" s="160" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="B13" s="137" t="s">
-        <v>1342</v>
-      </c>
-      <c r="C13" s="161" t="n">
+        <v>1340</v>
+      </c>
+      <c r="C13" s="160" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="B14" s="137" t="s">
-        <v>1344</v>
-      </c>
-      <c r="C14" s="161"/>
+        <v>1342</v>
+      </c>
+      <c r="C14" s="160"/>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="B15" s="137" t="s">
-        <v>1346</v>
-      </c>
-      <c r="C15" s="162" t="n">
+        <v>1344</v>
+      </c>
+      <c r="C15" s="161" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="B16" s="137" t="s">
-        <v>1348</v>
-      </c>
-      <c r="C16" s="162" t="n">
+        <v>1346</v>
+      </c>
+      <c r="C16" s="161" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="B17" s="137" t="s">
-        <v>1350</v>
-      </c>
-      <c r="C17" s="163" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C17" s="162" t="s">
         <v>932</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B18" s="137" t="s">
+        <v>1350</v>
+      </c>
+      <c r="C18" s="163" t="s">
         <v>1351</v>
       </c>
-      <c r="B18" s="137" t="s">
-        <v>1352</v>
-      </c>
-      <c r="C18" s="164" t="s">
-        <v>1353</v>
-      </c>
-      <c r="D18" s="165"/>
+      <c r="D18" s="164"/>
     </row>
     <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="B19" s="137" t="s">
-        <v>1355</v>
-      </c>
-      <c r="C19" s="163" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C19" s="162" t="s">
         <v>322</v>
       </c>
-      <c r="D19" s="165"/>
+      <c r="D19" s="164"/>
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B20" s="137" t="s">
-        <v>1357</v>
-      </c>
-      <c r="C20" s="163" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C20" s="162" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="B21" s="137" t="s">
-        <v>1359</v>
-      </c>
-      <c r="C21" s="164" t="n">
+        <v>1357</v>
+      </c>
+      <c r="C21" s="163" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="B22" s="137" t="s">
-        <v>1361</v>
-      </c>
-      <c r="C22" s="164" t="n">
+        <v>1359</v>
+      </c>
+      <c r="C22" s="163" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="B23" s="137" t="s">
-        <v>1363</v>
-      </c>
-      <c r="C23" s="164" t="n">
+        <v>1361</v>
+      </c>
+      <c r="C23" s="163" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B24" s="137" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C24" s="162" t="s">
         <v>1364</v>
       </c>
-      <c r="B24" s="137" t="s">
-        <v>1365</v>
-      </c>
-      <c r="C24" s="163" t="s">
-        <v>1366</v>
-      </c>
-      <c r="D24" s="166"/>
+      <c r="D24" s="165"/>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B25" s="137" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C25" s="162" t="s">
         <v>1367</v>
-      </c>
-      <c r="B25" s="137" t="s">
-        <v>1368</v>
-      </c>
-      <c r="C25" s="163" t="s">
-        <v>1369</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="B26" s="137" t="s">
-        <v>1371</v>
-      </c>
-      <c r="C26" s="162" t="n">
+        <v>1369</v>
+      </c>
+      <c r="C26" s="161" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B27" s="137" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C27" s="160" t="s">
         <v>1372</v>
-      </c>
-      <c r="B27" s="137" t="s">
-        <v>1373</v>
-      </c>
-      <c r="C27" s="161" t="s">
-        <v>1374</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="B28" s="137" t="s">
-        <v>1376</v>
-      </c>
-      <c r="C28" s="161" t="n">
+        <v>1374</v>
+      </c>
+      <c r="C28" s="160" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="B29" s="137" t="s">
-        <v>1378</v>
-      </c>
-      <c r="C29" s="162" t="n">
+        <v>1376</v>
+      </c>
+      <c r="C29" s="161" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="B30" s="137" t="s">
-        <v>1380</v>
-      </c>
-      <c r="C30" s="161"/>
+        <v>1378</v>
+      </c>
+      <c r="C30" s="160"/>
     </row>
   </sheetData>
   <dataValidations count="24">
@@ -28574,35 +28574,35 @@
   </cols>
   <sheetData>
     <row r="1" s="77" customFormat="true" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="167" t="s">
+      <c r="A1" s="166" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="167" t="s">
+      <c r="B1" s="166" t="s">
         <v>125</v>
       </c>
       <c r="C1" s="78" t="s">
+        <v>1379</v>
+      </c>
+      <c r="D1" s="78" t="s">
+        <v>1380</v>
+      </c>
+      <c r="E1" s="78" t="s">
         <v>1381</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="F1" s="77" t="s">
         <v>1382</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="G1" s="167" t="s">
         <v>1383</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="H1" s="78" t="s">
         <v>1384</v>
       </c>
-      <c r="G1" s="168" t="s">
+      <c r="I1" s="78" t="s">
         <v>1385</v>
       </c>
-      <c r="H1" s="78" t="s">
+      <c r="J1" s="78" t="s">
         <v>1386</v>
-      </c>
-      <c r="I1" s="78" t="s">
-        <v>1387</v>
-      </c>
-      <c r="J1" s="78" t="s">
-        <v>1388</v>
       </c>
       <c r="K1" s="78" t="s">
         <v>981</v>
@@ -28617,28 +28617,28 @@
         <v>184</v>
       </c>
       <c r="C2" s="137" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D2" s="137" t="s">
+        <v>1387</v>
+      </c>
+      <c r="E2" s="168" t="s">
+        <v>1388</v>
+      </c>
+      <c r="F2" s="137" t="s">
         <v>1389</v>
-      </c>
-      <c r="E2" s="169" t="s">
-        <v>1390</v>
-      </c>
-      <c r="F2" s="137" t="s">
-        <v>1391</v>
       </c>
       <c r="G2" s="137" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="137" t="s">
+        <v>1390</v>
+      </c>
+      <c r="I2" s="137" t="s">
+        <v>1391</v>
+      </c>
+      <c r="J2" s="137" t="s">
         <v>1392</v>
-      </c>
-      <c r="I2" s="137" t="s">
-        <v>1393</v>
-      </c>
-      <c r="J2" s="137" t="s">
-        <v>1394</v>
       </c>
       <c r="K2" s="137" t="s">
         <v>998</v>
@@ -28646,34 +28646,34 @@
     </row>
     <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>173</v>
       </c>
       <c r="C3" s="137" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="D3" s="137" t="s">
         <v>322</v>
       </c>
-      <c r="E3" s="169" t="s">
-        <v>1369</v>
+      <c r="E3" s="168" t="s">
+        <v>1367</v>
       </c>
       <c r="F3" s="137" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="G3" s="137" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="137" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="I3" s="137" t="s">
         <v>24</v>
       </c>
       <c r="J3" s="137" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="K3" s="137" t="s">
         <v>1006</v>
@@ -28681,21 +28681,21 @@
     </row>
     <row r="4" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="32" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>154</v>
       </c>
       <c r="C4" s="137" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="D4" s="137" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="F4" s="137" t="s">
-        <v>1366</v>
-      </c>
-      <c r="G4" s="169"/>
+        <v>1364</v>
+      </c>
+      <c r="G4" s="168"/>
       <c r="H4" s="137" t="s">
         <v>320</v>
       </c>
@@ -28707,16 +28707,16 @@
       <c r="B5" s="137" t="s">
         <v>206</v>
       </c>
-      <c r="G5" s="169"/>
+      <c r="G5" s="168"/>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>1404</v>
-      </c>
-      <c r="G6" s="169"/>
+        <v>1402</v>
+      </c>
+      <c r="G6" s="168"/>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="137" t="s">
@@ -28725,99 +28725,99 @@
       <c r="B7" s="137" t="s">
         <v>201</v>
       </c>
-      <c r="G7" s="169"/>
+      <c r="G7" s="168"/>
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="32" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>1404</v>
+      </c>
+      <c r="G8" s="168"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G9" s="168"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G10" s="168"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G11" s="168"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G12" s="168"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G13" s="168"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G14" s="168"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G15" s="168"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G16" s="168"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G17" s="168"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G18" s="168"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G19" s="168"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="169"/>
+      <c r="B20" s="169"/>
+      <c r="C20" s="169"/>
+      <c r="D20" s="169"/>
+      <c r="E20" s="170"/>
+      <c r="F20" s="169"/>
+      <c r="G20" s="170"/>
+      <c r="H20" s="169"/>
+      <c r="I20" s="169"/>
+      <c r="J20" s="169"/>
+      <c r="K20" s="169"/>
+      <c r="L20" s="169"/>
+    </row>
+    <row r="21" s="172" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="77" t="s">
         <v>1405</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B21" s="78" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C21" s="77" t="s">
         <v>1406</v>
       </c>
-      <c r="G8" s="169"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G9" s="169"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G10" s="169"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G11" s="169"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G12" s="169"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G13" s="169"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G14" s="169"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G15" s="169"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G16" s="169"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G17" s="169"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G18" s="169"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G19" s="169"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="170"/>
-      <c r="B20" s="170"/>
-      <c r="C20" s="170"/>
-      <c r="D20" s="170"/>
-      <c r="E20" s="171"/>
-      <c r="F20" s="170"/>
-      <c r="G20" s="171"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170"/>
-      <c r="J20" s="170"/>
-      <c r="K20" s="170"/>
-      <c r="L20" s="170"/>
-    </row>
-    <row r="21" s="173" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="77" t="s">
+      <c r="D21" s="77" t="s">
         <v>1407</v>
       </c>
-      <c r="B21" s="78" t="s">
-        <v>1328</v>
-      </c>
-      <c r="C21" s="77" t="s">
+      <c r="E21" s="171" t="s">
         <v>1408</v>
       </c>
-      <c r="D21" s="77" t="s">
+      <c r="F21" s="77" t="s">
         <v>1409</v>
       </c>
-      <c r="E21" s="172" t="s">
+      <c r="G21" s="77" t="s">
         <v>1410</v>
       </c>
-      <c r="F21" s="77" t="s">
+      <c r="H21" s="77" t="s">
         <v>1411</v>
       </c>
-      <c r="G21" s="77" t="s">
+      <c r="I21" s="77" t="s">
         <v>1412</v>
       </c>
-      <c r="H21" s="77" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="173" t="s">
         <v>1413</v>
       </c>
-      <c r="I21" s="77" t="s">
+      <c r="B22" s="137" t="s">
         <v>1414</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="174" t="s">
-        <v>1415</v>
-      </c>
-      <c r="B22" s="137" t="s">
-        <v>1416</v>
       </c>
       <c r="C22" s="137" t="s">
         <v>1137</v>
@@ -28825,11 +28825,11 @@
       <c r="D22" s="137" t="s">
         <v>1144</v>
       </c>
-      <c r="E22" s="169" t="s">
-        <v>1417</v>
+      <c r="E22" s="168" t="s">
+        <v>1415</v>
       </c>
       <c r="F22" s="137" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="G22" s="137" t="s">
         <v>893</v>
@@ -28843,19 +28843,19 @@
     </row>
     <row r="23" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="137" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C23" s="137" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D23" s="137" t="s">
+        <v>1319</v>
+      </c>
+      <c r="E23" s="168" t="s">
         <v>1419</v>
       </c>
-      <c r="C23" s="137" t="s">
+      <c r="F23" s="137" t="s">
         <v>1420</v>
-      </c>
-      <c r="D23" s="137" t="s">
-        <v>1321</v>
-      </c>
-      <c r="E23" s="169" t="s">
-        <v>1421</v>
-      </c>
-      <c r="F23" s="137" t="s">
-        <v>1422</v>
       </c>
       <c r="G23" s="137" t="s">
         <v>900</v>
@@ -28864,21 +28864,21 @@
         <v>900</v>
       </c>
       <c r="I23" s="137" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="137" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C24" s="137" t="s">
+        <v>1423</v>
+      </c>
+      <c r="D24" s="137" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F24" s="137" t="s">
         <v>1424</v>
-      </c>
-      <c r="C24" s="137" t="s">
-        <v>1425</v>
-      </c>
-      <c r="D24" s="137" t="s">
-        <v>1304</v>
-      </c>
-      <c r="F24" s="137" t="s">
-        <v>1426</v>
       </c>
       <c r="G24" s="137" t="s">
         <v>897</v>
@@ -28887,926 +28887,926 @@
         <v>897</v>
       </c>
       <c r="I24" s="137" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="137" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C25" s="137" t="s">
+        <v>1427</v>
+      </c>
+      <c r="D25" s="137" t="s">
+        <v>1320</v>
+      </c>
+      <c r="H25" s="137" t="s">
         <v>1428</v>
       </c>
-      <c r="C25" s="137" t="s">
+      <c r="I25" s="137" t="s">
         <v>1429</v>
-      </c>
-      <c r="D25" s="137" t="s">
-        <v>1322</v>
-      </c>
-      <c r="H25" s="137" t="s">
-        <v>1430</v>
-      </c>
-      <c r="I25" s="137" t="s">
-        <v>1431</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="137" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C26" s="137" t="s">
+        <v>1431</v>
+      </c>
+      <c r="H26" s="137" t="s">
         <v>1432</v>
-      </c>
-      <c r="C26" s="137" t="s">
-        <v>1433</v>
-      </c>
-      <c r="H26" s="137" t="s">
-        <v>1434</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="137" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="C27" s="137" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="137" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="137" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="137" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="C30" s="137" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="137" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="C31" s="137" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="137" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="C32" s="137" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="137" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="C33" s="137" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="137" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="137" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="137" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="137" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="137" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="137" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="137" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="137" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="137" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="137" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="137" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="137" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="137" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="137" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="137" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="137" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="137" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="137" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="137" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="137" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="137" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="137" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="137" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="137" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="137" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="137" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="137" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="137" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="137" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="137" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B64" s="137" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="137" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="137" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B67" s="137" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="137" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B69" s="137" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B70" s="137" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B71" s="137" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B72" s="137" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="137" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B74" s="137" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B75" s="137" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="137" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="137" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="137" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B79" s="137" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B80" s="137" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B81" s="137" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="137" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B83" s="137" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B84" s="137" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B85" s="137" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B86" s="137" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B87" s="137" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B88" s="137" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B89" s="137" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B90" s="137" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B91" s="137" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B92" s="137" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B93" s="137" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B94" s="137" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B95" s="137" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B96" s="137" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B97" s="137" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="137" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="137" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B100" s="137" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="137" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="137" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="137" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B104" s="137" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="137" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="137" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="137" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="137" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="137" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="137" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="137" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B112" s="137" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B113" s="137" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B114" s="137" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B115" s="137" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="137" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="137" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="137" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B119" s="137" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B120" s="137" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="137" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B122" s="137" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="137" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="137" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="137" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="137" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B127" s="137" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B128" s="137" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B129" s="137" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="137" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="137" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="137" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="137" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="137" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="137" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="137" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="137" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="137" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="137" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="137" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="137" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="137" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="137" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="137" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="137" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="137" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="137" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="137" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="137" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="137" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="137" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="137" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="137" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="137" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="137" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="137" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="137" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="137" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="137" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="137" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="137" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="137" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B163" s="137" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B164" s="137" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B165" s="137" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B166" s="137" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B167" s="137" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B168" s="137" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="137" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B170" s="137" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B171" s="137" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B172" s="137" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="137" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B174" s="137" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B175" s="137" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B176" s="137" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B177" s="137" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B178" s="137" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B179" s="137" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B180" s="137" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B181" s="137" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B182" s="137" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B183" s="137" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B184" s="137" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B185" s="137" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B186" s="137" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B187" s="137" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B188" s="137" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="137" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B190" s="137" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="137" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="137" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="137" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="137" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="137" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="137" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="137" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B198" s="137" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="137" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="137" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>